<commit_message>
Add new functionality to server -
adding COP/n_th Timeseries to Heat Generators
</commit_message>
<xml_diff>
--- a/app/modules/common/FEAT/F16/input.xlsx
+++ b/app/modules/common/FEAT/F16/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
   <si>
     <t>name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>prices(EUR/MWh)</t>
   </si>
   <si>
-    <t>emission factor</t>
-  </si>
-  <si>
     <t>ambient heat</t>
   </si>
   <si>
@@ -105,15 +102,9 @@
     <t>radiation</t>
   </si>
   <si>
-    <t>CO2 Price</t>
-  </si>
-  <si>
     <t>Interest Rate [0-1]</t>
   </si>
   <si>
-    <t>Total Renewable Factor [0-1]</t>
-  </si>
-  <si>
     <t>Total Demand[ MWh]</t>
   </si>
   <si>
@@ -132,15 +123,6 @@
     <t>unloading efficiency</t>
   </si>
   <si>
-    <t>Invesment costs for additional storage capacity  [€/MW]</t>
-  </si>
-  <si>
-    <t>Invesment costs for additional loading power  [€/MW]</t>
-  </si>
-  <si>
-    <t>OPEX fix [€/MWa]</t>
-  </si>
-  <si>
     <t>Life Time [a]</t>
   </si>
   <si>
@@ -253,6 +235,21 @@
   </si>
   <si>
     <t>Wasser-Wärmepumpe</t>
+  </si>
+  <si>
+    <t>emission factor [tCO2/MWh]</t>
+  </si>
+  <si>
+    <t>Minimum Renewable Factor [0-1]</t>
+  </si>
+  <si>
+    <t>CO2 Price [EUR/tC02]</t>
+  </si>
+  <si>
+    <t>Invesment costs for additional storage capacity  [€/MWh]</t>
+  </si>
+  <si>
+    <t>OPEX fix [€/MWha]</t>
   </si>
 </sst>
 </file>
@@ -336,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -350,6 +347,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -717,7 +720,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -747,10 +750,10 @@
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -758,10 +761,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>29</v>
@@ -788,7 +791,7 @@
         <v>0.5</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -797,10 +800,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>259</v>
@@ -827,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -836,10 +839,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -866,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -875,10 +878,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>169</v>
@@ -905,10 +908,10 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -916,10 +919,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>23</v>
@@ -946,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -954,10 +957,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>43</v>
@@ -984,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -992,10 +995,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>175</v>
@@ -1022,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1030,10 +1033,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D9">
         <v>95</v>
@@ -1066,10 +1069,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -1099,7 +1102,7 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1107,10 +1110,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1140,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1148,10 +1151,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1181,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1194,7 +1197,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,13 +1211,13 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1222,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1239,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>0.3</v>
@@ -1256,7 +1259,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1273,7 +1276,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>0.3</v>
@@ -1290,7 +1293,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>0.2</v>
@@ -1307,7 +1310,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1324,7 +1327,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1341,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>0.12</v>
@@ -1358,7 +1361,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1375,7 +1378,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1392,7 +1395,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1409,7 +1412,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1426,7 +1429,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1448,7 +1451,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1492,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>62</v>
@@ -1517,7 +1520,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>47</v>
@@ -1534,7 +1537,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -1551,7 +1554,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>22</v>
@@ -1568,7 +1571,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -1585,7 +1588,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -1602,7 +1605,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1619,7 +1622,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1636,7 +1639,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1653,7 +1656,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>36</v>
@@ -1670,7 +1673,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1692,7 +1695,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,16 +1706,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1773,52 +1776,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1835,16 +1846,13 @@
       <c r="G2">
         <v>0.98</v>
       </c>
-      <c r="H2">
-        <v>3000</v>
-      </c>
-      <c r="I2">
-        <v>75000</v>
+      <c r="H2" s="7">
+        <v>60</v>
+      </c>
+      <c r="I2" s="7">
+        <v>10000</v>
       </c>
       <c r="J2">
-        <v>10000</v>
-      </c>
-      <c r="K2">
         <v>25</v>
       </c>
     </row>
@@ -1872,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1880,10 +1888,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1891,10 +1899,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1902,10 +1910,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1913,10 +1921,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1924,10 +1932,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1935,10 +1943,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1946,10 +1954,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1957,10 +1965,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1968,10 +1976,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1979,10 +1987,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,10 +1998,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2019,19 +2027,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,19 +2047,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2059,19 +2067,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2079,19 +2087,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>